<commit_message>
added draft 1 of reviews
</commit_message>
<xml_diff>
--- a/man/Project_Plan/group_members.xlsx
+++ b/man/Project_Plan/group_members.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Role</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Calvin Chan</t>
   </si>
   <si>
-    <t>Qa</t>
-  </si>
-  <si>
     <t>Karl Franks</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>Scott Lockett</t>
   </si>
   <si>
-    <t>WebApp</t>
-  </si>
-  <si>
     <t>Kieran Lynch</t>
   </si>
   <si>
@@ -87,18 +81,6 @@
     <t>Zach Yewman</t>
   </si>
   <si>
-    <t>Testing team</t>
-  </si>
-  <si>
-    <t>Project lead / sorta DB master</t>
-  </si>
-  <si>
-    <t>Qa/testing team</t>
-  </si>
-  <si>
-    <t>Server team</t>
-  </si>
-  <si>
     <t>Android team</t>
   </si>
   <si>
@@ -109,13 +91,43 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>QA / Testing team lead</t>
+  </si>
+  <si>
+    <t>QA / Testing team</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Web-Team</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>Web-Team Lead</t>
+  </si>
+  <si>
+    <t>QA team</t>
+  </si>
+  <si>
+    <t>Project lead / Database</t>
+  </si>
+  <si>
+    <t>QA (reviews) / Documentation</t>
+  </si>
+  <si>
+    <t>Documentation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -124,22 +136,46 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD7EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -149,10 +185,12 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
       <top/>
       <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FFFFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -160,22 +198,104 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -189,17 +309,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B26" totalsRowShown="0">
-  <autoFilter ref="A1:B26"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Role"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -465,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,215 +589,220 @@
     <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="12" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>